<commit_message>
Commit Jornada 6 Final
</commit_message>
<xml_diff>
--- a/SALAMANCA UDS 2324.xlsx
+++ b/SALAMANCA UDS 2324.xlsx
@@ -1888,6 +1888,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1900,16 +1912,22 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1919,24 +1937,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2545,42 +2545,42 @@
       </c>
     </row>
     <row r="3" spans="2:24" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="139" t="s">
+      <c r="B3" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="140"/>
-      <c r="H3" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="139" t="s">
+      <c r="F3" s="136"/>
+      <c r="H3" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="140"/>
-      <c r="N3" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="138"/>
-      <c r="P3" s="138"/>
-      <c r="Q3" s="139" t="s">
+      <c r="L3" s="136"/>
+      <c r="N3" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="140"/>
-      <c r="T3" s="133" t="s">
-        <v>0</v>
-      </c>
-      <c r="U3" s="134"/>
-      <c r="V3" s="134"/>
-      <c r="W3" s="135" t="s">
+      <c r="R3" s="136"/>
+      <c r="T3" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="138"/>
+      <c r="V3" s="138"/>
+      <c r="W3" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="136"/>
+      <c r="X3" s="140"/>
     </row>
     <row r="4" spans="2:24" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
@@ -3916,18 +3916,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27248,192 +27248,192 @@
       <c r="AF2" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="AH2" s="141" t="s">
+      <c r="AH2" s="147" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" s="142"/>
-      <c r="AJ2" s="142"/>
-      <c r="AK2" s="142"/>
-      <c r="AL2" s="142"/>
-      <c r="AM2" s="142"/>
-      <c r="AN2" s="143"/>
-      <c r="AP2" s="141" t="s">
+      <c r="AI2" s="148"/>
+      <c r="AJ2" s="148"/>
+      <c r="AK2" s="148"/>
+      <c r="AL2" s="148"/>
+      <c r="AM2" s="148"/>
+      <c r="AN2" s="149"/>
+      <c r="AP2" s="147" t="s">
         <v>34</v>
       </c>
-      <c r="AQ2" s="142"/>
-      <c r="AR2" s="142"/>
-      <c r="AS2" s="142"/>
-      <c r="AT2" s="142"/>
-      <c r="AU2" s="142"/>
-      <c r="AV2" s="143"/>
-      <c r="AX2" s="141" t="s">
+      <c r="AQ2" s="148"/>
+      <c r="AR2" s="148"/>
+      <c r="AS2" s="148"/>
+      <c r="AT2" s="148"/>
+      <c r="AU2" s="148"/>
+      <c r="AV2" s="149"/>
+      <c r="AX2" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="AY2" s="142"/>
-      <c r="AZ2" s="142"/>
-      <c r="BA2" s="142"/>
-      <c r="BB2" s="142"/>
-      <c r="BC2" s="142"/>
-      <c r="BD2" s="143"/>
-      <c r="BF2" s="141" t="s">
+      <c r="AY2" s="148"/>
+      <c r="AZ2" s="148"/>
+      <c r="BA2" s="148"/>
+      <c r="BB2" s="148"/>
+      <c r="BC2" s="148"/>
+      <c r="BD2" s="149"/>
+      <c r="BF2" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="BG2" s="142"/>
-      <c r="BH2" s="142"/>
-      <c r="BI2" s="142"/>
-      <c r="BJ2" s="142"/>
-      <c r="BK2" s="142"/>
-      <c r="BL2" s="143"/>
-      <c r="BN2" s="141" t="s">
+      <c r="BG2" s="148"/>
+      <c r="BH2" s="148"/>
+      <c r="BI2" s="148"/>
+      <c r="BJ2" s="148"/>
+      <c r="BK2" s="148"/>
+      <c r="BL2" s="149"/>
+      <c r="BN2" s="147" t="s">
         <v>37</v>
       </c>
-      <c r="BO2" s="142"/>
-      <c r="BP2" s="142"/>
-      <c r="BQ2" s="142"/>
-      <c r="BR2" s="142"/>
-      <c r="BS2" s="142"/>
-      <c r="BT2" s="143"/>
-      <c r="BV2" s="141" t="s">
+      <c r="BO2" s="148"/>
+      <c r="BP2" s="148"/>
+      <c r="BQ2" s="148"/>
+      <c r="BR2" s="148"/>
+      <c r="BS2" s="148"/>
+      <c r="BT2" s="149"/>
+      <c r="BV2" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="BW2" s="142"/>
-      <c r="BX2" s="142"/>
-      <c r="BY2" s="142"/>
-      <c r="BZ2" s="142"/>
-      <c r="CA2" s="142"/>
-      <c r="CB2" s="143"/>
+      <c r="BW2" s="148"/>
+      <c r="BX2" s="148"/>
+      <c r="BY2" s="148"/>
+      <c r="BZ2" s="148"/>
+      <c r="CA2" s="148"/>
+      <c r="CB2" s="149"/>
     </row>
     <row r="3" spans="2:80" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="149" t="s">
+      <c r="B3" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="149"/>
-      <c r="G3" s="139" t="s">
+      <c r="F3" s="146"/>
+      <c r="G3" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="140"/>
-      <c r="J3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="144" t="s">
+      <c r="H3" s="136"/>
+      <c r="J3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="144"/>
-      <c r="O3" s="145" t="s">
+      <c r="N3" s="145"/>
+      <c r="O3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="146"/>
-      <c r="R3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="148"/>
-      <c r="T3" s="148"/>
-      <c r="U3" s="144" t="s">
+      <c r="P3" s="144"/>
+      <c r="R3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="142"/>
+      <c r="T3" s="142"/>
+      <c r="U3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="144"/>
-      <c r="W3" s="145" t="s">
+      <c r="V3" s="145"/>
+      <c r="W3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="146"/>
-      <c r="Z3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="148"/>
-      <c r="AB3" s="148"/>
-      <c r="AC3" s="144" t="s">
+      <c r="X3" s="144"/>
+      <c r="Z3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="142"/>
+      <c r="AB3" s="142"/>
+      <c r="AC3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="144"/>
-      <c r="AE3" s="145" t="s">
+      <c r="AD3" s="145"/>
+      <c r="AE3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AF3" s="146"/>
-      <c r="AH3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="148"/>
-      <c r="AJ3" s="148"/>
-      <c r="AK3" s="144" t="s">
+      <c r="AF3" s="144"/>
+      <c r="AH3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="142"/>
+      <c r="AJ3" s="142"/>
+      <c r="AK3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AL3" s="144"/>
-      <c r="AM3" s="145" t="s">
+      <c r="AL3" s="145"/>
+      <c r="AM3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AN3" s="146"/>
-      <c r="AP3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="148"/>
-      <c r="AR3" s="148"/>
-      <c r="AS3" s="144" t="s">
+      <c r="AN3" s="144"/>
+      <c r="AP3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="142"/>
+      <c r="AR3" s="142"/>
+      <c r="AS3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AT3" s="144"/>
-      <c r="AU3" s="145" t="s">
+      <c r="AT3" s="145"/>
+      <c r="AU3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AV3" s="146"/>
-      <c r="AX3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="148"/>
-      <c r="AZ3" s="148"/>
-      <c r="BA3" s="144" t="s">
+      <c r="AV3" s="144"/>
+      <c r="AX3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="142"/>
+      <c r="AZ3" s="142"/>
+      <c r="BA3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BB3" s="144"/>
-      <c r="BC3" s="145" t="s">
+      <c r="BB3" s="145"/>
+      <c r="BC3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BD3" s="146"/>
-      <c r="BF3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BG3" s="148"/>
-      <c r="BH3" s="148"/>
-      <c r="BI3" s="144" t="s">
+      <c r="BD3" s="144"/>
+      <c r="BF3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="142"/>
+      <c r="BH3" s="142"/>
+      <c r="BI3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BJ3" s="144"/>
-      <c r="BK3" s="145" t="s">
+      <c r="BJ3" s="145"/>
+      <c r="BK3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BL3" s="146"/>
-      <c r="BN3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BO3" s="148"/>
-      <c r="BP3" s="148"/>
-      <c r="BQ3" s="144" t="s">
+      <c r="BL3" s="144"/>
+      <c r="BN3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="142"/>
+      <c r="BP3" s="142"/>
+      <c r="BQ3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BR3" s="144"/>
-      <c r="BS3" s="145" t="s">
+      <c r="BR3" s="145"/>
+      <c r="BS3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BT3" s="146"/>
-      <c r="BV3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BW3" s="148"/>
-      <c r="BX3" s="148"/>
-      <c r="BY3" s="144" t="s">
+      <c r="BT3" s="144"/>
+      <c r="BV3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW3" s="142"/>
+      <c r="BX3" s="142"/>
+      <c r="BY3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BZ3" s="144"/>
-      <c r="CA3" s="145" t="s">
+      <c r="BZ3" s="145"/>
+      <c r="CA3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CB3" s="146"/>
+      <c r="CB3" s="144"/>
     </row>
     <row r="4" spans="2:80" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
@@ -29951,24 +29951,12 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="CA3:CB3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BN3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="BV3:BX3"/>
-    <mergeCell ref="BY3:BZ3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="S2:W2"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="BF2:BL2"/>
+    <mergeCell ref="AA2:AE2"/>
     <mergeCell ref="BN2:BT2"/>
     <mergeCell ref="BV2:CB2"/>
     <mergeCell ref="AH2:AN2"/>
@@ -29985,12 +29973,24 @@
     <mergeCell ref="AX3:AZ3"/>
     <mergeCell ref="BA3:BB3"/>
     <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="S2:W2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BF2:BL2"/>
-    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="CA3:CB3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BN3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BS3:BT3"/>
+    <mergeCell ref="BV3:BX3"/>
+    <mergeCell ref="BY3:BZ3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31237,19 +31237,19 @@
       <c r="L39" s="152"/>
     </row>
     <row r="40" spans="6:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="F40" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" s="148"/>
-      <c r="H40" s="148"/>
-      <c r="I40" s="144" t="s">
+      <c r="F40" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="142"/>
+      <c r="H40" s="142"/>
+      <c r="I40" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="J40" s="144"/>
-      <c r="K40" s="145" t="s">
+      <c r="J40" s="145"/>
+      <c r="K40" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="L40" s="146"/>
+      <c r="L40" s="144"/>
     </row>
     <row r="41" spans="6:23" ht="19" x14ac:dyDescent="0.25">
       <c r="F41" s="14" t="s">
@@ -31927,8 +31927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:EF25"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AR26" sqref="AR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32099,328 +32099,328 @@
       <c r="AV2" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="AX2" s="141" t="s">
+      <c r="AX2" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="AY2" s="142"/>
-      <c r="AZ2" s="142"/>
-      <c r="BA2" s="142"/>
-      <c r="BB2" s="142"/>
-      <c r="BC2" s="142"/>
-      <c r="BD2" s="143"/>
-      <c r="BF2" s="141" t="s">
+      <c r="AY2" s="148"/>
+      <c r="AZ2" s="148"/>
+      <c r="BA2" s="148"/>
+      <c r="BB2" s="148"/>
+      <c r="BC2" s="148"/>
+      <c r="BD2" s="149"/>
+      <c r="BF2" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="BG2" s="142"/>
-      <c r="BH2" s="142"/>
-      <c r="BI2" s="142"/>
-      <c r="BJ2" s="142"/>
-      <c r="BK2" s="142"/>
-      <c r="BL2" s="143"/>
-      <c r="BN2" s="141" t="s">
+      <c r="BG2" s="148"/>
+      <c r="BH2" s="148"/>
+      <c r="BI2" s="148"/>
+      <c r="BJ2" s="148"/>
+      <c r="BK2" s="148"/>
+      <c r="BL2" s="149"/>
+      <c r="BN2" s="147" t="s">
         <v>37</v>
       </c>
-      <c r="BO2" s="142"/>
-      <c r="BP2" s="142"/>
-      <c r="BQ2" s="142"/>
-      <c r="BR2" s="142"/>
-      <c r="BS2" s="142"/>
-      <c r="BT2" s="143"/>
-      <c r="BV2" s="141" t="s">
+      <c r="BO2" s="148"/>
+      <c r="BP2" s="148"/>
+      <c r="BQ2" s="148"/>
+      <c r="BR2" s="148"/>
+      <c r="BS2" s="148"/>
+      <c r="BT2" s="149"/>
+      <c r="BV2" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="BW2" s="142"/>
-      <c r="BX2" s="142"/>
-      <c r="BY2" s="142"/>
-      <c r="BZ2" s="142"/>
-      <c r="CA2" s="142"/>
-      <c r="CB2" s="143"/>
-      <c r="CD2" s="141" t="s">
+      <c r="BW2" s="148"/>
+      <c r="BX2" s="148"/>
+      <c r="BY2" s="148"/>
+      <c r="BZ2" s="148"/>
+      <c r="CA2" s="148"/>
+      <c r="CB2" s="149"/>
+      <c r="CD2" s="147" t="s">
         <v>39</v>
       </c>
-      <c r="CE2" s="142"/>
-      <c r="CF2" s="142"/>
-      <c r="CG2" s="142"/>
-      <c r="CH2" s="142"/>
-      <c r="CI2" s="142"/>
-      <c r="CJ2" s="143"/>
-      <c r="CL2" s="141" t="s">
+      <c r="CE2" s="148"/>
+      <c r="CF2" s="148"/>
+      <c r="CG2" s="148"/>
+      <c r="CH2" s="148"/>
+      <c r="CI2" s="148"/>
+      <c r="CJ2" s="149"/>
+      <c r="CL2" s="147" t="s">
         <v>40</v>
       </c>
-      <c r="CM2" s="142"/>
-      <c r="CN2" s="142"/>
-      <c r="CO2" s="142"/>
-      <c r="CP2" s="142"/>
-      <c r="CQ2" s="142"/>
-      <c r="CR2" s="143"/>
-      <c r="CT2" s="141" t="s">
+      <c r="CM2" s="148"/>
+      <c r="CN2" s="148"/>
+      <c r="CO2" s="148"/>
+      <c r="CP2" s="148"/>
+      <c r="CQ2" s="148"/>
+      <c r="CR2" s="149"/>
+      <c r="CT2" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="CU2" s="142"/>
-      <c r="CV2" s="142"/>
-      <c r="CW2" s="142"/>
-      <c r="CX2" s="142"/>
-      <c r="CY2" s="142"/>
-      <c r="CZ2" s="143"/>
-      <c r="DB2" s="141" t="s">
+      <c r="CU2" s="148"/>
+      <c r="CV2" s="148"/>
+      <c r="CW2" s="148"/>
+      <c r="CX2" s="148"/>
+      <c r="CY2" s="148"/>
+      <c r="CZ2" s="149"/>
+      <c r="DB2" s="147" t="s">
         <v>45</v>
       </c>
-      <c r="DC2" s="142"/>
-      <c r="DD2" s="142"/>
-      <c r="DE2" s="142"/>
-      <c r="DF2" s="142"/>
-      <c r="DG2" s="142"/>
-      <c r="DH2" s="143"/>
-      <c r="DJ2" s="141" t="s">
+      <c r="DC2" s="148"/>
+      <c r="DD2" s="148"/>
+      <c r="DE2" s="148"/>
+      <c r="DF2" s="148"/>
+      <c r="DG2" s="148"/>
+      <c r="DH2" s="149"/>
+      <c r="DJ2" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="DK2" s="142"/>
-      <c r="DL2" s="142"/>
-      <c r="DM2" s="142"/>
-      <c r="DN2" s="142"/>
-      <c r="DO2" s="142"/>
-      <c r="DP2" s="143"/>
-      <c r="DR2" s="141" t="s">
+      <c r="DK2" s="148"/>
+      <c r="DL2" s="148"/>
+      <c r="DM2" s="148"/>
+      <c r="DN2" s="148"/>
+      <c r="DO2" s="148"/>
+      <c r="DP2" s="149"/>
+      <c r="DR2" s="147" t="s">
         <v>43</v>
       </c>
-      <c r="DS2" s="142"/>
-      <c r="DT2" s="142"/>
-      <c r="DU2" s="142"/>
-      <c r="DV2" s="142"/>
-      <c r="DW2" s="142"/>
-      <c r="DX2" s="143"/>
-      <c r="DZ2" s="141" t="s">
+      <c r="DS2" s="148"/>
+      <c r="DT2" s="148"/>
+      <c r="DU2" s="148"/>
+      <c r="DV2" s="148"/>
+      <c r="DW2" s="148"/>
+      <c r="DX2" s="149"/>
+      <c r="DZ2" s="147" t="s">
         <v>42</v>
       </c>
-      <c r="EA2" s="142"/>
-      <c r="EB2" s="142"/>
-      <c r="EC2" s="142"/>
-      <c r="ED2" s="142"/>
-      <c r="EE2" s="142"/>
-      <c r="EF2" s="143"/>
+      <c r="EA2" s="148"/>
+      <c r="EB2" s="148"/>
+      <c r="EC2" s="148"/>
+      <c r="ED2" s="148"/>
+      <c r="EE2" s="148"/>
+      <c r="EF2" s="149"/>
     </row>
     <row r="3" spans="2:136" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="144" t="s">
+      <c r="B3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="144"/>
-      <c r="G3" s="145" t="s">
+      <c r="F3" s="145"/>
+      <c r="G3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="146"/>
-      <c r="J3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="144" t="s">
+      <c r="H3" s="144"/>
+      <c r="J3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="144"/>
-      <c r="O3" s="145" t="s">
+      <c r="N3" s="145"/>
+      <c r="O3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="146"/>
-      <c r="R3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="148"/>
-      <c r="T3" s="148"/>
-      <c r="U3" s="144" t="s">
+      <c r="P3" s="144"/>
+      <c r="R3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="142"/>
+      <c r="T3" s="142"/>
+      <c r="U3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="144"/>
-      <c r="W3" s="145" t="s">
+      <c r="V3" s="145"/>
+      <c r="W3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="146"/>
-      <c r="Z3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="148"/>
-      <c r="AB3" s="148"/>
-      <c r="AC3" s="144" t="s">
+      <c r="X3" s="144"/>
+      <c r="Z3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="142"/>
+      <c r="AB3" s="142"/>
+      <c r="AC3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="144"/>
-      <c r="AE3" s="145" t="s">
+      <c r="AD3" s="145"/>
+      <c r="AE3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AF3" s="146"/>
-      <c r="AH3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="148"/>
-      <c r="AJ3" s="148"/>
-      <c r="AK3" s="144" t="s">
+      <c r="AF3" s="144"/>
+      <c r="AH3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="142"/>
+      <c r="AJ3" s="142"/>
+      <c r="AK3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AL3" s="144"/>
-      <c r="AM3" s="145" t="s">
+      <c r="AL3" s="145"/>
+      <c r="AM3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AN3" s="146"/>
-      <c r="AP3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="148"/>
-      <c r="AR3" s="148"/>
-      <c r="AS3" s="144" t="s">
+      <c r="AN3" s="144"/>
+      <c r="AP3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="142"/>
+      <c r="AR3" s="142"/>
+      <c r="AS3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AT3" s="144"/>
-      <c r="AU3" s="145" t="s">
+      <c r="AT3" s="145"/>
+      <c r="AU3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AV3" s="146"/>
-      <c r="AX3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="148"/>
-      <c r="AZ3" s="148"/>
-      <c r="BA3" s="144" t="s">
+      <c r="AV3" s="144"/>
+      <c r="AX3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="142"/>
+      <c r="AZ3" s="142"/>
+      <c r="BA3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BB3" s="144"/>
-      <c r="BC3" s="145" t="s">
+      <c r="BB3" s="145"/>
+      <c r="BC3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BD3" s="146"/>
-      <c r="BF3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BG3" s="148"/>
-      <c r="BH3" s="148"/>
-      <c r="BI3" s="144" t="s">
+      <c r="BD3" s="144"/>
+      <c r="BF3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="142"/>
+      <c r="BH3" s="142"/>
+      <c r="BI3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BJ3" s="144"/>
-      <c r="BK3" s="145" t="s">
+      <c r="BJ3" s="145"/>
+      <c r="BK3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BL3" s="146"/>
-      <c r="BN3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BO3" s="148"/>
-      <c r="BP3" s="148"/>
-      <c r="BQ3" s="144" t="s">
+      <c r="BL3" s="144"/>
+      <c r="BN3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="142"/>
+      <c r="BP3" s="142"/>
+      <c r="BQ3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BR3" s="144"/>
-      <c r="BS3" s="145" t="s">
+      <c r="BR3" s="145"/>
+      <c r="BS3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BT3" s="146"/>
-      <c r="BV3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BW3" s="148"/>
-      <c r="BX3" s="148"/>
-      <c r="BY3" s="144" t="s">
+      <c r="BT3" s="144"/>
+      <c r="BV3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW3" s="142"/>
+      <c r="BX3" s="142"/>
+      <c r="BY3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BZ3" s="144"/>
-      <c r="CA3" s="145" t="s">
+      <c r="BZ3" s="145"/>
+      <c r="CA3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CB3" s="146"/>
-      <c r="CD3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE3" s="148"/>
-      <c r="CF3" s="148"/>
-      <c r="CG3" s="144" t="s">
+      <c r="CB3" s="144"/>
+      <c r="CD3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE3" s="142"/>
+      <c r="CF3" s="142"/>
+      <c r="CG3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="CH3" s="144"/>
-      <c r="CI3" s="145" t="s">
+      <c r="CH3" s="145"/>
+      <c r="CI3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CJ3" s="146"/>
-      <c r="CL3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="CM3" s="148"/>
-      <c r="CN3" s="148"/>
-      <c r="CO3" s="144" t="s">
+      <c r="CJ3" s="144"/>
+      <c r="CL3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM3" s="142"/>
+      <c r="CN3" s="142"/>
+      <c r="CO3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="CP3" s="144"/>
-      <c r="CQ3" s="145" t="s">
+      <c r="CP3" s="145"/>
+      <c r="CQ3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CR3" s="146"/>
-      <c r="CT3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="CU3" s="148"/>
-      <c r="CV3" s="148"/>
-      <c r="CW3" s="144" t="s">
+      <c r="CR3" s="144"/>
+      <c r="CT3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU3" s="142"/>
+      <c r="CV3" s="142"/>
+      <c r="CW3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="CX3" s="144"/>
-      <c r="CY3" s="145" t="s">
+      <c r="CX3" s="145"/>
+      <c r="CY3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CZ3" s="146"/>
-      <c r="DB3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="DC3" s="148"/>
-      <c r="DD3" s="148"/>
-      <c r="DE3" s="144" t="s">
+      <c r="CZ3" s="144"/>
+      <c r="DB3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="DC3" s="142"/>
+      <c r="DD3" s="142"/>
+      <c r="DE3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="DF3" s="144"/>
-      <c r="DG3" s="145" t="s">
+      <c r="DF3" s="145"/>
+      <c r="DG3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="DH3" s="146"/>
-      <c r="DJ3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="DK3" s="148"/>
-      <c r="DL3" s="148"/>
-      <c r="DM3" s="144" t="s">
+      <c r="DH3" s="144"/>
+      <c r="DJ3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="DK3" s="142"/>
+      <c r="DL3" s="142"/>
+      <c r="DM3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="DN3" s="144"/>
-      <c r="DO3" s="145" t="s">
+      <c r="DN3" s="145"/>
+      <c r="DO3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="DP3" s="146"/>
-      <c r="DR3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="DS3" s="148"/>
-      <c r="DT3" s="148"/>
-      <c r="DU3" s="144" t="s">
+      <c r="DP3" s="144"/>
+      <c r="DR3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="DS3" s="142"/>
+      <c r="DT3" s="142"/>
+      <c r="DU3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="DV3" s="144"/>
-      <c r="DW3" s="145" t="s">
+      <c r="DV3" s="145"/>
+      <c r="DW3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="DX3" s="146"/>
-      <c r="DZ3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="EA3" s="148"/>
-      <c r="EB3" s="148"/>
-      <c r="EC3" s="144" t="s">
+      <c r="DX3" s="144"/>
+      <c r="DZ3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="EA3" s="142"/>
+      <c r="EB3" s="142"/>
+      <c r="EC3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="ED3" s="144"/>
-      <c r="EE3" s="145" t="s">
+      <c r="ED3" s="145"/>
+      <c r="EE3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="EF3" s="146"/>
+      <c r="EF3" s="144"/>
     </row>
     <row r="4" spans="2:136" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
@@ -32853,7 +32853,9 @@
       <c r="AQ5" s="7">
         <v>1</v>
       </c>
-      <c r="AR5" s="7"/>
+      <c r="AR5" s="7">
+        <v>90</v>
+      </c>
       <c r="AS5" s="7"/>
       <c r="AT5" s="7"/>
       <c r="AU5" s="7"/>
@@ -33692,7 +33694,9 @@
       <c r="AQ10" s="7">
         <v>1</v>
       </c>
-      <c r="AR10" s="7"/>
+      <c r="AR10" s="7">
+        <v>90</v>
+      </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="7"/>
       <c r="AU10" s="7"/>
@@ -34219,7 +34223,9 @@
       <c r="AQ13" s="7">
         <v>1</v>
       </c>
-      <c r="AR13" s="7"/>
+      <c r="AR13" s="7">
+        <v>90</v>
+      </c>
       <c r="AS13" s="7"/>
       <c r="AT13" s="7"/>
       <c r="AU13" s="7"/>
@@ -35084,7 +35090,9 @@
       <c r="AQ18" s="7">
         <v>1</v>
       </c>
-      <c r="AR18" s="7"/>
+      <c r="AR18" s="7">
+        <v>90</v>
+      </c>
       <c r="AS18" s="7"/>
       <c r="AT18" s="7"/>
       <c r="AU18" s="7"/>
@@ -35609,7 +35617,9 @@
       <c r="AQ21" s="7">
         <v>1</v>
       </c>
-      <c r="AR21" s="7"/>
+      <c r="AR21" s="7">
+        <v>90</v>
+      </c>
       <c r="AS21" s="7"/>
       <c r="AT21" s="7"/>
       <c r="AU21" s="7"/>
@@ -35965,7 +35975,9 @@
       <c r="AQ23" s="7">
         <v>1</v>
       </c>
-      <c r="AR23" s="7"/>
+      <c r="AR23" s="7">
+        <v>90</v>
+      </c>
       <c r="AS23" s="7">
         <v>1</v>
       </c>
@@ -36246,9 +36258,69 @@
         <f>SUM(AB5:AB24)</f>
         <v>990</v>
       </c>
+      <c r="AR25">
+        <f>SUM(AR5:AR23)</f>
+        <v>990</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AI2:AM2"/>
+    <mergeCell ref="AQ2:AU2"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="S2:W2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BF2:BL2"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BI3:BJ3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BN2:BT2"/>
+    <mergeCell ref="BN3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BS3:BT3"/>
+    <mergeCell ref="BV2:CB2"/>
+    <mergeCell ref="BV3:BX3"/>
+    <mergeCell ref="BY3:BZ3"/>
+    <mergeCell ref="CA3:CB3"/>
+    <mergeCell ref="CD2:CJ2"/>
+    <mergeCell ref="CD3:CF3"/>
+    <mergeCell ref="CG3:CH3"/>
+    <mergeCell ref="CI3:CJ3"/>
+    <mergeCell ref="CL2:CR2"/>
+    <mergeCell ref="CL3:CN3"/>
+    <mergeCell ref="CO3:CP3"/>
+    <mergeCell ref="CQ3:CR3"/>
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="CT3:CV3"/>
+    <mergeCell ref="CW3:CX3"/>
+    <mergeCell ref="CY3:CZ3"/>
+    <mergeCell ref="DB2:DH2"/>
+    <mergeCell ref="DB3:DD3"/>
+    <mergeCell ref="DE3:DF3"/>
+    <mergeCell ref="DG3:DH3"/>
     <mergeCell ref="DZ2:EF2"/>
     <mergeCell ref="DZ3:EB3"/>
     <mergeCell ref="EC3:ED3"/>
@@ -36261,62 +36333,6 @@
     <mergeCell ref="DR3:DT3"/>
     <mergeCell ref="DU3:DV3"/>
     <mergeCell ref="DW3:DX3"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="CT3:CV3"/>
-    <mergeCell ref="CW3:CX3"/>
-    <mergeCell ref="CY3:CZ3"/>
-    <mergeCell ref="DB2:DH2"/>
-    <mergeCell ref="DB3:DD3"/>
-    <mergeCell ref="DE3:DF3"/>
-    <mergeCell ref="DG3:DH3"/>
-    <mergeCell ref="CD2:CJ2"/>
-    <mergeCell ref="CD3:CF3"/>
-    <mergeCell ref="CG3:CH3"/>
-    <mergeCell ref="CI3:CJ3"/>
-    <mergeCell ref="CL2:CR2"/>
-    <mergeCell ref="CL3:CN3"/>
-    <mergeCell ref="CO3:CP3"/>
-    <mergeCell ref="CQ3:CR3"/>
-    <mergeCell ref="BN2:BT2"/>
-    <mergeCell ref="BN3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="BV2:CB2"/>
-    <mergeCell ref="BV3:BX3"/>
-    <mergeCell ref="BY3:BZ3"/>
-    <mergeCell ref="CA3:CB3"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="AX3:AZ3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BF2:BL2"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BI3:BJ3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AI2:AM2"/>
-    <mergeCell ref="AQ2:AU2"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="S2:W2"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36405,7 +36421,7 @@
       </c>
       <c r="F3" s="8">
         <f>'1º Vuelta'!D5+'1º Vuelta'!L5+'1º Vuelta'!T5+'1º Vuelta'!AB5+'1º Vuelta'!AJ5+'1º Vuelta'!AR5+'1º Vuelta'!AZ5+'1º Vuelta'!BH5+'1º Vuelta'!BP5+'1º Vuelta'!BX5+'1º Vuelta'!CF5+'1º Vuelta'!CN5+'1º Vuelta'!CV5+'1º Vuelta'!DD5+'1º Vuelta'!DL5+'1º Vuelta'!DT5+'1º Vuelta'!EB5</f>
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>10</v>
@@ -36655,7 +36671,7 @@
       </c>
       <c r="F8" s="8">
         <f>'1º Vuelta'!D10+'1º Vuelta'!L10+'1º Vuelta'!T10+'1º Vuelta'!AB10+'1º Vuelta'!AJ10+'1º Vuelta'!AR10+'1º Vuelta'!AZ10+'1º Vuelta'!BH10+'1º Vuelta'!BP10+'1º Vuelta'!BX10+'1º Vuelta'!CF10+'1º Vuelta'!CN10+'1º Vuelta'!CV10+'1º Vuelta'!DD10+'1º Vuelta'!DL10+'1º Vuelta'!DT10+'1º Vuelta'!EB10</f>
-        <v>439</v>
+        <v>529</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>15</v>
@@ -36805,7 +36821,7 @@
       </c>
       <c r="F11" s="8">
         <f>'1º Vuelta'!D13+'1º Vuelta'!L13+'1º Vuelta'!T13+'1º Vuelta'!AB13+'1º Vuelta'!AJ13+'1º Vuelta'!AR13+'1º Vuelta'!AZ13+'1º Vuelta'!BH13+'1º Vuelta'!BP13+'1º Vuelta'!BX13+'1º Vuelta'!CF13+'1º Vuelta'!CN13+'1º Vuelta'!CV13+'1º Vuelta'!DD13+'1º Vuelta'!DL13+'1º Vuelta'!DT13+'1º Vuelta'!EB13</f>
-        <v>370</v>
+        <v>460</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>18</v>
@@ -37050,7 +37066,7 @@
       </c>
       <c r="F16" s="8">
         <f>'1º Vuelta'!D18+'1º Vuelta'!L18+'1º Vuelta'!T18+'1º Vuelta'!AB18+'1º Vuelta'!AJ18+'1º Vuelta'!AR18+'1º Vuelta'!AZ18+'1º Vuelta'!BH18+'1º Vuelta'!BP18+'1º Vuelta'!BX18+'1º Vuelta'!CF18+'1º Vuelta'!CN18+'1º Vuelta'!CV18+'1º Vuelta'!DD18+'1º Vuelta'!DL18+'1º Vuelta'!DT18+'1º Vuelta'!EB18</f>
-        <v>428</v>
+        <v>518</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>24</v>
@@ -37200,7 +37216,7 @@
       </c>
       <c r="F19" s="8">
         <f>'1º Vuelta'!D21+'1º Vuelta'!L21+'1º Vuelta'!T21+'1º Vuelta'!AB21+'1º Vuelta'!AJ21+'1º Vuelta'!AR21+'1º Vuelta'!AZ21+'1º Vuelta'!BH21+'1º Vuelta'!BP21+'1º Vuelta'!BX21+'1º Vuelta'!CF21+'1º Vuelta'!CN21+'1º Vuelta'!CV21+'1º Vuelta'!DD21+'1º Vuelta'!DL21+'1º Vuelta'!DT21+'1º Vuelta'!EB21</f>
-        <v>319</v>
+        <v>409</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>27</v>
@@ -37300,7 +37316,7 @@
       </c>
       <c r="F21" s="8">
         <f>'1º Vuelta'!D23+'1º Vuelta'!L23+'1º Vuelta'!T23+'1º Vuelta'!AB23+'1º Vuelta'!AJ23+'1º Vuelta'!AR23+'1º Vuelta'!AZ23+'1º Vuelta'!BH23+'1º Vuelta'!BP23+'1º Vuelta'!BX23+'1º Vuelta'!CF23+'1º Vuelta'!CN23+'1º Vuelta'!CV23+'1º Vuelta'!DD23+'1º Vuelta'!DL23+'1º Vuelta'!DT23+'1º Vuelta'!EB23</f>
-        <v>365</v>
+        <v>455</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>29</v>
@@ -37475,30 +37491,30 @@
     </row>
     <row r="36" spans="5:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="5:22" ht="19" x14ac:dyDescent="0.25">
-      <c r="E37" s="141" t="s">
+      <c r="E37" s="147" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="142"/>
-      <c r="G37" s="142"/>
-      <c r="H37" s="142"/>
-      <c r="I37" s="142"/>
-      <c r="J37" s="142"/>
-      <c r="K37" s="143"/>
+      <c r="F37" s="148"/>
+      <c r="G37" s="148"/>
+      <c r="H37" s="148"/>
+      <c r="I37" s="148"/>
+      <c r="J37" s="148"/>
+      <c r="K37" s="149"/>
     </row>
     <row r="38" spans="5:22" ht="19" x14ac:dyDescent="0.25">
-      <c r="E38" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="F38" s="148"/>
-      <c r="G38" s="148"/>
-      <c r="H38" s="144" t="s">
+      <c r="E38" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="142"/>
+      <c r="G38" s="142"/>
+      <c r="H38" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="I38" s="144"/>
-      <c r="J38" s="145" t="s">
+      <c r="I38" s="145"/>
+      <c r="J38" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="K38" s="146"/>
+      <c r="K38" s="144"/>
     </row>
     <row r="39" spans="5:22" ht="19" x14ac:dyDescent="0.25">
       <c r="E39" s="14" t="s">
@@ -37533,7 +37549,7 @@
       </c>
       <c r="G40" s="7">
         <f>'1º Vuelta'!D5+'1º Vuelta'!L5+'1º Vuelta'!T5+'1º Vuelta'!AB5+'1º Vuelta'!AJ5+'1º Vuelta'!AR5+'1º Vuelta'!AZ5+'1º Vuelta'!BH5+'1º Vuelta'!BP5+'1º Vuelta'!BX5+'1º Vuelta'!CF5+'1º Vuelta'!CN5+'1º Vuelta'!CV5+'1º Vuelta'!DD5+'1º Vuelta'!DL5+'1º Vuelta'!DT5+'1º Vuelta'!EB5</f>
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="H40" s="7">
         <f>'1º Vuelta'!E5+'1º Vuelta'!M5+'1º Vuelta'!U5+'1º Vuelta'!AC5+'1º Vuelta'!AK5+'1º Vuelta'!AS5+'1º Vuelta'!BA5+'1º Vuelta'!BI5+'1º Vuelta'!BQ5+'1º Vuelta'!BY5+'1º Vuelta'!CG5+'1º Vuelta'!CO5+'1º Vuelta'!CW5+'1º Vuelta'!DE5+'1º Vuelta'!DM5+'1º Vuelta'!DU5+'1º Vuelta'!EC5</f>
@@ -37678,7 +37694,7 @@
       </c>
       <c r="G45" s="7">
         <f>'1º Vuelta'!D10+'1º Vuelta'!L10+'1º Vuelta'!T10+'1º Vuelta'!AB10+'1º Vuelta'!AJ10+'1º Vuelta'!AR10+'1º Vuelta'!AZ10+'1º Vuelta'!BH10+'1º Vuelta'!BP10+'1º Vuelta'!BX10+'1º Vuelta'!CF10+'1º Vuelta'!CN10+'1º Vuelta'!CV10+'1º Vuelta'!DD10+'1º Vuelta'!DL10+'1º Vuelta'!DT10+'1º Vuelta'!EB10</f>
-        <v>439</v>
+        <v>529</v>
       </c>
       <c r="H45" s="7">
         <f>'1º Vuelta'!E10+'1º Vuelta'!M10+'1º Vuelta'!U10+'1º Vuelta'!AC10+'1º Vuelta'!AK10+'1º Vuelta'!AS10+'1º Vuelta'!BA10+'1º Vuelta'!BI10+'1º Vuelta'!BQ10+'1º Vuelta'!BY10+'1º Vuelta'!CG10+'1º Vuelta'!CO10+'1º Vuelta'!CW10+'1º Vuelta'!DE10+'1º Vuelta'!DM10+'1º Vuelta'!DU10+'1º Vuelta'!EC10</f>
@@ -37765,7 +37781,7 @@
       </c>
       <c r="G48" s="7">
         <f>'1º Vuelta'!D13+'1º Vuelta'!L13+'1º Vuelta'!T13+'1º Vuelta'!AB13+'1º Vuelta'!AJ13+'1º Vuelta'!AR13+'1º Vuelta'!AZ13+'1º Vuelta'!BH13+'1º Vuelta'!BP13+'1º Vuelta'!BX13+'1º Vuelta'!CF13+'1º Vuelta'!CN13+'1º Vuelta'!CV13+'1º Vuelta'!DD13+'1º Vuelta'!DL13+'1º Vuelta'!DT13+'1º Vuelta'!EB13</f>
-        <v>370</v>
+        <v>460</v>
       </c>
       <c r="H48" s="7">
         <f>'1º Vuelta'!E13+'1º Vuelta'!M13+'1º Vuelta'!U13+'1º Vuelta'!AC13+'1º Vuelta'!AK13+'1º Vuelta'!AS13+'1º Vuelta'!BA13+'1º Vuelta'!BI13+'1º Vuelta'!BQ13+'1º Vuelta'!BY13+'1º Vuelta'!CG13+'1º Vuelta'!CO13+'1º Vuelta'!CW13+'1º Vuelta'!DE13+'1º Vuelta'!DM13+'1º Vuelta'!DU13+'1º Vuelta'!EC13</f>
@@ -37910,7 +37926,7 @@
       </c>
       <c r="G53" s="7">
         <f>'1º Vuelta'!D18+'1º Vuelta'!L18+'1º Vuelta'!T18+'1º Vuelta'!AB18+'1º Vuelta'!AJ18+'1º Vuelta'!AR18+'1º Vuelta'!AZ18+'1º Vuelta'!BH18+'1º Vuelta'!BP18+'1º Vuelta'!BX18+'1º Vuelta'!CF18+'1º Vuelta'!CN18+'1º Vuelta'!CV18+'1º Vuelta'!DD18+'1º Vuelta'!DL18+'1º Vuelta'!DT18+'1º Vuelta'!EB18</f>
-        <v>428</v>
+        <v>518</v>
       </c>
       <c r="H53" s="7">
         <f>'1º Vuelta'!E18+'1º Vuelta'!M18+'1º Vuelta'!U18+'1º Vuelta'!AC18+'1º Vuelta'!AK18+'1º Vuelta'!AS18+'1º Vuelta'!BA18+'1º Vuelta'!BI18+'1º Vuelta'!BQ18+'1º Vuelta'!BY18+'1º Vuelta'!CG18+'1º Vuelta'!CO18+'1º Vuelta'!CW18+'1º Vuelta'!DE18+'1º Vuelta'!DM18+'1º Vuelta'!DU18+'1º Vuelta'!EC18</f>
@@ -37997,7 +38013,7 @@
       </c>
       <c r="G56" s="7">
         <f>'1º Vuelta'!D21+'1º Vuelta'!L21+'1º Vuelta'!T21+'1º Vuelta'!AB21+'1º Vuelta'!AJ21+'1º Vuelta'!AR21+'1º Vuelta'!AZ21+'1º Vuelta'!BH21+'1º Vuelta'!BP21+'1º Vuelta'!BX21+'1º Vuelta'!CF21+'1º Vuelta'!CN21+'1º Vuelta'!CV21+'1º Vuelta'!DD21+'1º Vuelta'!DL21+'1º Vuelta'!DT21+'1º Vuelta'!EB21</f>
-        <v>319</v>
+        <v>409</v>
       </c>
       <c r="H56" s="7">
         <f>'1º Vuelta'!E21+'1º Vuelta'!M21+'1º Vuelta'!U21+'1º Vuelta'!AC21+'1º Vuelta'!AK21+'1º Vuelta'!AS21+'1º Vuelta'!BA21+'1º Vuelta'!BI21+'1º Vuelta'!BQ21+'1º Vuelta'!BY21+'1º Vuelta'!CG21+'1º Vuelta'!CO21+'1º Vuelta'!CW21+'1º Vuelta'!DE21+'1º Vuelta'!DM21+'1º Vuelta'!DU21+'1º Vuelta'!EC21</f>
@@ -38055,7 +38071,7 @@
       </c>
       <c r="G58" s="7">
         <f>'1º Vuelta'!D23+'1º Vuelta'!L23+'1º Vuelta'!T23+'1º Vuelta'!AB23+'1º Vuelta'!AJ23+'1º Vuelta'!AR23+'1º Vuelta'!AZ23+'1º Vuelta'!BH23+'1º Vuelta'!BP23+'1º Vuelta'!BX23+'1º Vuelta'!CF23+'1º Vuelta'!CN23+'1º Vuelta'!CV23+'1º Vuelta'!DD23+'1º Vuelta'!DL23+'1º Vuelta'!DT23+'1º Vuelta'!EB23</f>
-        <v>365</v>
+        <v>455</v>
       </c>
       <c r="H58" s="7">
         <f>'1º Vuelta'!E23+'1º Vuelta'!M23+'1º Vuelta'!U23+'1º Vuelta'!AC23+'1º Vuelta'!AK23+'1º Vuelta'!AS23+'1º Vuelta'!BA23+'1º Vuelta'!BI23+'1º Vuelta'!BQ23+'1º Vuelta'!BY23+'1º Vuelta'!CG23+'1º Vuelta'!CO23+'1º Vuelta'!CW23+'1º Vuelta'!DE23+'1º Vuelta'!DM23+'1º Vuelta'!DU23+'1º Vuelta'!EC23</f>
@@ -38215,382 +38231,382 @@
   <sheetData>
     <row r="1" spans="2:136" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:136" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="141" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="143"/>
-      <c r="J2" s="141" t="s">
+      <c r="B2" s="147" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="149"/>
+      <c r="J2" s="147" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="142"/>
-      <c r="O2" s="142"/>
-      <c r="P2" s="143"/>
-      <c r="R2" s="141" t="s">
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
+      <c r="M2" s="148"/>
+      <c r="N2" s="148"/>
+      <c r="O2" s="148"/>
+      <c r="P2" s="149"/>
+      <c r="R2" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="142"/>
-      <c r="T2" s="142"/>
-      <c r="U2" s="142"/>
-      <c r="V2" s="142"/>
-      <c r="W2" s="142"/>
-      <c r="X2" s="143"/>
-      <c r="Z2" s="141" t="s">
+      <c r="S2" s="148"/>
+      <c r="T2" s="148"/>
+      <c r="U2" s="148"/>
+      <c r="V2" s="148"/>
+      <c r="W2" s="148"/>
+      <c r="X2" s="149"/>
+      <c r="Z2" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="142"/>
-      <c r="AB2" s="142"/>
-      <c r="AC2" s="142"/>
-      <c r="AD2" s="142"/>
-      <c r="AE2" s="142"/>
-      <c r="AF2" s="143"/>
-      <c r="AH2" s="141" t="s">
+      <c r="AA2" s="148"/>
+      <c r="AB2" s="148"/>
+      <c r="AC2" s="148"/>
+      <c r="AD2" s="148"/>
+      <c r="AE2" s="148"/>
+      <c r="AF2" s="149"/>
+      <c r="AH2" s="147" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" s="142"/>
-      <c r="AJ2" s="142"/>
-      <c r="AK2" s="142"/>
-      <c r="AL2" s="142"/>
-      <c r="AM2" s="142"/>
-      <c r="AN2" s="143"/>
-      <c r="AP2" s="141" t="s">
+      <c r="AI2" s="148"/>
+      <c r="AJ2" s="148"/>
+      <c r="AK2" s="148"/>
+      <c r="AL2" s="148"/>
+      <c r="AM2" s="148"/>
+      <c r="AN2" s="149"/>
+      <c r="AP2" s="147" t="s">
         <v>34</v>
       </c>
-      <c r="AQ2" s="142"/>
-      <c r="AR2" s="142"/>
-      <c r="AS2" s="142"/>
-      <c r="AT2" s="142"/>
-      <c r="AU2" s="142"/>
-      <c r="AV2" s="143"/>
-      <c r="AX2" s="141" t="s">
+      <c r="AQ2" s="148"/>
+      <c r="AR2" s="148"/>
+      <c r="AS2" s="148"/>
+      <c r="AT2" s="148"/>
+      <c r="AU2" s="148"/>
+      <c r="AV2" s="149"/>
+      <c r="AX2" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="AY2" s="142"/>
-      <c r="AZ2" s="142"/>
-      <c r="BA2" s="142"/>
-      <c r="BB2" s="142"/>
-      <c r="BC2" s="142"/>
-      <c r="BD2" s="143"/>
-      <c r="BF2" s="141" t="s">
+      <c r="AY2" s="148"/>
+      <c r="AZ2" s="148"/>
+      <c r="BA2" s="148"/>
+      <c r="BB2" s="148"/>
+      <c r="BC2" s="148"/>
+      <c r="BD2" s="149"/>
+      <c r="BF2" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="BG2" s="142"/>
-      <c r="BH2" s="142"/>
-      <c r="BI2" s="142"/>
-      <c r="BJ2" s="142"/>
-      <c r="BK2" s="142"/>
-      <c r="BL2" s="143"/>
-      <c r="BN2" s="141" t="s">
+      <c r="BG2" s="148"/>
+      <c r="BH2" s="148"/>
+      <c r="BI2" s="148"/>
+      <c r="BJ2" s="148"/>
+      <c r="BK2" s="148"/>
+      <c r="BL2" s="149"/>
+      <c r="BN2" s="147" t="s">
         <v>37</v>
       </c>
-      <c r="BO2" s="142"/>
-      <c r="BP2" s="142"/>
-      <c r="BQ2" s="142"/>
-      <c r="BR2" s="142"/>
-      <c r="BS2" s="142"/>
-      <c r="BT2" s="143"/>
-      <c r="BV2" s="141" t="s">
+      <c r="BO2" s="148"/>
+      <c r="BP2" s="148"/>
+      <c r="BQ2" s="148"/>
+      <c r="BR2" s="148"/>
+      <c r="BS2" s="148"/>
+      <c r="BT2" s="149"/>
+      <c r="BV2" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="BW2" s="142"/>
-      <c r="BX2" s="142"/>
-      <c r="BY2" s="142"/>
-      <c r="BZ2" s="142"/>
-      <c r="CA2" s="142"/>
-      <c r="CB2" s="143"/>
-      <c r="CD2" s="141" t="s">
+      <c r="BW2" s="148"/>
+      <c r="BX2" s="148"/>
+      <c r="BY2" s="148"/>
+      <c r="BZ2" s="148"/>
+      <c r="CA2" s="148"/>
+      <c r="CB2" s="149"/>
+      <c r="CD2" s="147" t="s">
         <v>39</v>
       </c>
-      <c r="CE2" s="142"/>
-      <c r="CF2" s="142"/>
-      <c r="CG2" s="142"/>
-      <c r="CH2" s="142"/>
-      <c r="CI2" s="142"/>
-      <c r="CJ2" s="143"/>
-      <c r="CL2" s="141" t="s">
+      <c r="CE2" s="148"/>
+      <c r="CF2" s="148"/>
+      <c r="CG2" s="148"/>
+      <c r="CH2" s="148"/>
+      <c r="CI2" s="148"/>
+      <c r="CJ2" s="149"/>
+      <c r="CL2" s="147" t="s">
         <v>40</v>
       </c>
-      <c r="CM2" s="142"/>
-      <c r="CN2" s="142"/>
-      <c r="CO2" s="142"/>
-      <c r="CP2" s="142"/>
-      <c r="CQ2" s="142"/>
-      <c r="CR2" s="143"/>
-      <c r="CT2" s="141" t="s">
+      <c r="CM2" s="148"/>
+      <c r="CN2" s="148"/>
+      <c r="CO2" s="148"/>
+      <c r="CP2" s="148"/>
+      <c r="CQ2" s="148"/>
+      <c r="CR2" s="149"/>
+      <c r="CT2" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="CU2" s="142"/>
-      <c r="CV2" s="142"/>
-      <c r="CW2" s="142"/>
-      <c r="CX2" s="142"/>
-      <c r="CY2" s="142"/>
-      <c r="CZ2" s="143"/>
-      <c r="DB2" s="141" t="s">
+      <c r="CU2" s="148"/>
+      <c r="CV2" s="148"/>
+      <c r="CW2" s="148"/>
+      <c r="CX2" s="148"/>
+      <c r="CY2" s="148"/>
+      <c r="CZ2" s="149"/>
+      <c r="DB2" s="147" t="s">
         <v>45</v>
       </c>
-      <c r="DC2" s="142"/>
-      <c r="DD2" s="142"/>
-      <c r="DE2" s="142"/>
-      <c r="DF2" s="142"/>
-      <c r="DG2" s="142"/>
-      <c r="DH2" s="143"/>
-      <c r="DJ2" s="141" t="s">
+      <c r="DC2" s="148"/>
+      <c r="DD2" s="148"/>
+      <c r="DE2" s="148"/>
+      <c r="DF2" s="148"/>
+      <c r="DG2" s="148"/>
+      <c r="DH2" s="149"/>
+      <c r="DJ2" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="DK2" s="142"/>
-      <c r="DL2" s="142"/>
-      <c r="DM2" s="142"/>
-      <c r="DN2" s="142"/>
-      <c r="DO2" s="142"/>
-      <c r="DP2" s="143"/>
-      <c r="DR2" s="141" t="s">
+      <c r="DK2" s="148"/>
+      <c r="DL2" s="148"/>
+      <c r="DM2" s="148"/>
+      <c r="DN2" s="148"/>
+      <c r="DO2" s="148"/>
+      <c r="DP2" s="149"/>
+      <c r="DR2" s="147" t="s">
         <v>43</v>
       </c>
-      <c r="DS2" s="142"/>
-      <c r="DT2" s="142"/>
-      <c r="DU2" s="142"/>
-      <c r="DV2" s="142"/>
-      <c r="DW2" s="142"/>
-      <c r="DX2" s="143"/>
-      <c r="DZ2" s="141" t="s">
+      <c r="DS2" s="148"/>
+      <c r="DT2" s="148"/>
+      <c r="DU2" s="148"/>
+      <c r="DV2" s="148"/>
+      <c r="DW2" s="148"/>
+      <c r="DX2" s="149"/>
+      <c r="DZ2" s="147" t="s">
         <v>42</v>
       </c>
-      <c r="EA2" s="142"/>
-      <c r="EB2" s="142"/>
-      <c r="EC2" s="142"/>
-      <c r="ED2" s="142"/>
-      <c r="EE2" s="142"/>
-      <c r="EF2" s="143"/>
+      <c r="EA2" s="148"/>
+      <c r="EB2" s="148"/>
+      <c r="EC2" s="148"/>
+      <c r="ED2" s="148"/>
+      <c r="EE2" s="148"/>
+      <c r="EF2" s="149"/>
     </row>
     <row r="3" spans="2:136" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="144" t="s">
+      <c r="B3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="144"/>
-      <c r="G3" s="145" t="s">
+      <c r="F3" s="145"/>
+      <c r="G3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="146"/>
-      <c r="J3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="144" t="s">
+      <c r="H3" s="144"/>
+      <c r="J3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="144"/>
-      <c r="O3" s="145" t="s">
+      <c r="N3" s="145"/>
+      <c r="O3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="146"/>
-      <c r="R3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="148"/>
-      <c r="T3" s="148"/>
-      <c r="U3" s="144" t="s">
+      <c r="P3" s="144"/>
+      <c r="R3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="142"/>
+      <c r="T3" s="142"/>
+      <c r="U3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="144"/>
-      <c r="W3" s="145" t="s">
+      <c r="V3" s="145"/>
+      <c r="W3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="146"/>
-      <c r="Z3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="148"/>
-      <c r="AB3" s="148"/>
-      <c r="AC3" s="144" t="s">
+      <c r="X3" s="144"/>
+      <c r="Z3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="142"/>
+      <c r="AB3" s="142"/>
+      <c r="AC3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="144"/>
-      <c r="AE3" s="145" t="s">
+      <c r="AD3" s="145"/>
+      <c r="AE3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AF3" s="146"/>
-      <c r="AH3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="148"/>
-      <c r="AJ3" s="148"/>
-      <c r="AK3" s="144" t="s">
+      <c r="AF3" s="144"/>
+      <c r="AH3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="142"/>
+      <c r="AJ3" s="142"/>
+      <c r="AK3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AL3" s="144"/>
-      <c r="AM3" s="145" t="s">
+      <c r="AL3" s="145"/>
+      <c r="AM3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AN3" s="146"/>
-      <c r="AP3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="148"/>
-      <c r="AR3" s="148"/>
-      <c r="AS3" s="144" t="s">
+      <c r="AN3" s="144"/>
+      <c r="AP3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="142"/>
+      <c r="AR3" s="142"/>
+      <c r="AS3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="AT3" s="144"/>
-      <c r="AU3" s="145" t="s">
+      <c r="AT3" s="145"/>
+      <c r="AU3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="AV3" s="146"/>
-      <c r="AX3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="148"/>
-      <c r="AZ3" s="148"/>
-      <c r="BA3" s="144" t="s">
+      <c r="AV3" s="144"/>
+      <c r="AX3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="142"/>
+      <c r="AZ3" s="142"/>
+      <c r="BA3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BB3" s="144"/>
-      <c r="BC3" s="145" t="s">
+      <c r="BB3" s="145"/>
+      <c r="BC3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BD3" s="146"/>
-      <c r="BF3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BG3" s="148"/>
-      <c r="BH3" s="148"/>
-      <c r="BI3" s="144" t="s">
+      <c r="BD3" s="144"/>
+      <c r="BF3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="142"/>
+      <c r="BH3" s="142"/>
+      <c r="BI3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BJ3" s="144"/>
-      <c r="BK3" s="145" t="s">
+      <c r="BJ3" s="145"/>
+      <c r="BK3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BL3" s="146"/>
-      <c r="BN3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BO3" s="148"/>
-      <c r="BP3" s="148"/>
-      <c r="BQ3" s="144" t="s">
+      <c r="BL3" s="144"/>
+      <c r="BN3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="142"/>
+      <c r="BP3" s="142"/>
+      <c r="BQ3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BR3" s="144"/>
-      <c r="BS3" s="145" t="s">
+      <c r="BR3" s="145"/>
+      <c r="BS3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="BT3" s="146"/>
-      <c r="BV3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="BW3" s="148"/>
-      <c r="BX3" s="148"/>
-      <c r="BY3" s="144" t="s">
+      <c r="BT3" s="144"/>
+      <c r="BV3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW3" s="142"/>
+      <c r="BX3" s="142"/>
+      <c r="BY3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="BZ3" s="144"/>
-      <c r="CA3" s="145" t="s">
+      <c r="BZ3" s="145"/>
+      <c r="CA3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CB3" s="146"/>
-      <c r="CD3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE3" s="148"/>
-      <c r="CF3" s="148"/>
-      <c r="CG3" s="144" t="s">
+      <c r="CB3" s="144"/>
+      <c r="CD3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE3" s="142"/>
+      <c r="CF3" s="142"/>
+      <c r="CG3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="CH3" s="144"/>
-      <c r="CI3" s="145" t="s">
+      <c r="CH3" s="145"/>
+      <c r="CI3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CJ3" s="146"/>
-      <c r="CL3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="CM3" s="148"/>
-      <c r="CN3" s="148"/>
-      <c r="CO3" s="144" t="s">
+      <c r="CJ3" s="144"/>
+      <c r="CL3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM3" s="142"/>
+      <c r="CN3" s="142"/>
+      <c r="CO3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="CP3" s="144"/>
-      <c r="CQ3" s="145" t="s">
+      <c r="CP3" s="145"/>
+      <c r="CQ3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CR3" s="146"/>
-      <c r="CT3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="CU3" s="148"/>
-      <c r="CV3" s="148"/>
-      <c r="CW3" s="144" t="s">
+      <c r="CR3" s="144"/>
+      <c r="CT3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU3" s="142"/>
+      <c r="CV3" s="142"/>
+      <c r="CW3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="CX3" s="144"/>
-      <c r="CY3" s="145" t="s">
+      <c r="CX3" s="145"/>
+      <c r="CY3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="CZ3" s="146"/>
-      <c r="DB3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="DC3" s="148"/>
-      <c r="DD3" s="148"/>
-      <c r="DE3" s="144" t="s">
+      <c r="CZ3" s="144"/>
+      <c r="DB3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="DC3" s="142"/>
+      <c r="DD3" s="142"/>
+      <c r="DE3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="DF3" s="144"/>
-      <c r="DG3" s="145" t="s">
+      <c r="DF3" s="145"/>
+      <c r="DG3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="DH3" s="146"/>
-      <c r="DJ3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="DK3" s="148"/>
-      <c r="DL3" s="148"/>
-      <c r="DM3" s="144" t="s">
+      <c r="DH3" s="144"/>
+      <c r="DJ3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="DK3" s="142"/>
+      <c r="DL3" s="142"/>
+      <c r="DM3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="DN3" s="144"/>
-      <c r="DO3" s="145" t="s">
+      <c r="DN3" s="145"/>
+      <c r="DO3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="DP3" s="146"/>
-      <c r="DR3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="DS3" s="148"/>
-      <c r="DT3" s="148"/>
-      <c r="DU3" s="144" t="s">
+      <c r="DP3" s="144"/>
+      <c r="DR3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="DS3" s="142"/>
+      <c r="DT3" s="142"/>
+      <c r="DU3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="DV3" s="144"/>
-      <c r="DW3" s="145" t="s">
+      <c r="DV3" s="145"/>
+      <c r="DW3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="DX3" s="146"/>
-      <c r="DZ3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="EA3" s="148"/>
-      <c r="EB3" s="148"/>
-      <c r="EC3" s="144" t="s">
+      <c r="DX3" s="144"/>
+      <c r="DZ3" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="EA3" s="142"/>
+      <c r="EB3" s="142"/>
+      <c r="EC3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="ED3" s="144"/>
-      <c r="EE3" s="145" t="s">
+      <c r="ED3" s="145"/>
+      <c r="EE3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="EF3" s="146"/>
+      <c r="EF3" s="144"/>
     </row>
     <row r="4" spans="2:136" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
@@ -42363,16 +42379,52 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="DW3:DX3"/>
-    <mergeCell ref="DZ3:EB3"/>
-    <mergeCell ref="EC3:ED3"/>
-    <mergeCell ref="EE3:EF3"/>
-    <mergeCell ref="DG3:DH3"/>
-    <mergeCell ref="DJ3:DL3"/>
-    <mergeCell ref="DM3:DN3"/>
-    <mergeCell ref="DO3:DP3"/>
-    <mergeCell ref="DR3:DT3"/>
-    <mergeCell ref="DU3:DV3"/>
+    <mergeCell ref="CL2:CR2"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="Z2:AF2"/>
+    <mergeCell ref="AH2:AN2"/>
+    <mergeCell ref="AP2:AV2"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="BF2:BL2"/>
+    <mergeCell ref="BN2:BT2"/>
+    <mergeCell ref="BV2:CB2"/>
+    <mergeCell ref="CD2:CJ2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="DB2:DH2"/>
+    <mergeCell ref="DJ2:DP2"/>
+    <mergeCell ref="DR2:DX2"/>
+    <mergeCell ref="DZ2:EF2"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="BY3:BZ3"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BI3:BJ3"/>
+    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="BN3:BP3"/>
+    <mergeCell ref="BQ3:BR3"/>
+    <mergeCell ref="BS3:BT3"/>
+    <mergeCell ref="BV3:BX3"/>
     <mergeCell ref="DE3:DF3"/>
     <mergeCell ref="CA3:CB3"/>
     <mergeCell ref="CD3:CF3"/>
@@ -42385,52 +42437,16 @@
     <mergeCell ref="CW3:CX3"/>
     <mergeCell ref="CY3:CZ3"/>
     <mergeCell ref="DB3:DD3"/>
-    <mergeCell ref="BY3:BZ3"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AX3:AZ3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BI3:BJ3"/>
-    <mergeCell ref="BK3:BL3"/>
-    <mergeCell ref="BN3:BP3"/>
-    <mergeCell ref="BQ3:BR3"/>
-    <mergeCell ref="BS3:BT3"/>
-    <mergeCell ref="BV3:BX3"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="DB2:DH2"/>
-    <mergeCell ref="DJ2:DP2"/>
-    <mergeCell ref="DR2:DX2"/>
-    <mergeCell ref="DZ2:EF2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="CL2:CR2"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="Z2:AF2"/>
-    <mergeCell ref="AH2:AN2"/>
-    <mergeCell ref="AP2:AV2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BF2:BL2"/>
-    <mergeCell ref="BN2:BT2"/>
-    <mergeCell ref="BV2:CB2"/>
-    <mergeCell ref="CD2:CJ2"/>
+    <mergeCell ref="DW3:DX3"/>
+    <mergeCell ref="DZ3:EB3"/>
+    <mergeCell ref="EC3:ED3"/>
+    <mergeCell ref="EE3:EF3"/>
+    <mergeCell ref="DG3:DH3"/>
+    <mergeCell ref="DJ3:DL3"/>
+    <mergeCell ref="DM3:DN3"/>
+    <mergeCell ref="DO3:DP3"/>
+    <mergeCell ref="DR3:DT3"/>
+    <mergeCell ref="DU3:DV3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43308,30 +43324,30 @@
     </row>
     <row r="38" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="3:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="C39" s="141" t="s">
+      <c r="C39" s="147" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="142"/>
-      <c r="E39" s="142"/>
-      <c r="F39" s="142"/>
-      <c r="G39" s="142"/>
-      <c r="H39" s="142"/>
-      <c r="I39" s="143"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="148"/>
+      <c r="H39" s="148"/>
+      <c r="I39" s="149"/>
     </row>
     <row r="40" spans="3:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="C40" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="148"/>
-      <c r="E40" s="148"/>
-      <c r="F40" s="144" t="s">
+      <c r="C40" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="142"/>
+      <c r="E40" s="142"/>
+      <c r="F40" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="144"/>
-      <c r="H40" s="145" t="s">
+      <c r="G40" s="145"/>
+      <c r="H40" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="I40" s="146"/>
+      <c r="I40" s="144"/>
     </row>
     <row r="41" spans="3:9" ht="19" x14ac:dyDescent="0.25">
       <c r="C41" s="14" t="s">
@@ -44085,7 +44101,7 @@
       </c>
       <c r="G3" s="8">
         <f t="shared" ref="G3:G24" si="0">H42</f>
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>10</v>
@@ -44305,7 +44321,7 @@
       </c>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
-        <v>439</v>
+        <v>529</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>15</v>
@@ -44437,7 +44453,7 @@
       </c>
       <c r="G11" s="8">
         <f t="shared" si="0"/>
-        <v>370</v>
+        <v>460</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>18</v>
@@ -44701,7 +44717,7 @@
       </c>
       <c r="G17" s="8">
         <f t="shared" si="0"/>
-        <v>428</v>
+        <v>518</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>24</v>
@@ -44833,7 +44849,7 @@
       </c>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
-        <v>319</v>
+        <v>409</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>27</v>
@@ -44921,7 +44937,7 @@
       </c>
       <c r="G22" s="8">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>455</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>29</v>
@@ -45053,19 +45069,19 @@
       <c r="L39" s="152"/>
     </row>
     <row r="40" spans="6:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="F40" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" s="148"/>
-      <c r="H40" s="148"/>
-      <c r="I40" s="144" t="s">
+      <c r="F40" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="142"/>
+      <c r="H40" s="142"/>
+      <c r="I40" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="J40" s="144"/>
-      <c r="K40" s="145" t="s">
+      <c r="J40" s="145"/>
+      <c r="K40" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="L40" s="146"/>
+      <c r="L40" s="144"/>
     </row>
     <row r="41" spans="6:12" ht="19" x14ac:dyDescent="0.25">
       <c r="F41" s="14" t="s">
@@ -45100,7 +45116,7 @@
       </c>
       <c r="H42" s="7">
         <f>'Estadisticas 1º Vuelta'!G40+'Estadisticas 2º Vuelta'!E42</f>
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="I42" s="7">
         <f>'Estadisticas 1º Vuelta'!H40+'Estadisticas 2º Vuelta'!F42</f>
@@ -45245,7 +45261,7 @@
       </c>
       <c r="H47" s="7">
         <f>'Estadisticas 1º Vuelta'!G45+'Estadisticas 2º Vuelta'!E47</f>
-        <v>439</v>
+        <v>529</v>
       </c>
       <c r="I47" s="7">
         <f>'Estadisticas 1º Vuelta'!H45+'Estadisticas 2º Vuelta'!F47</f>
@@ -45332,7 +45348,7 @@
       </c>
       <c r="H50" s="7">
         <f>'Estadisticas 1º Vuelta'!G48+'Estadisticas 2º Vuelta'!E50</f>
-        <v>370</v>
+        <v>460</v>
       </c>
       <c r="I50" s="7">
         <f>'Estadisticas 1º Vuelta'!H48+'Estadisticas 2º Vuelta'!F50</f>
@@ -45506,7 +45522,7 @@
       </c>
       <c r="H56" s="7">
         <f>'Estadisticas 1º Vuelta'!G53+'Estadisticas 2º Vuelta'!E56</f>
-        <v>428</v>
+        <v>518</v>
       </c>
       <c r="I56" s="7">
         <f>'Estadisticas 1º Vuelta'!H53+'Estadisticas 2º Vuelta'!F56</f>
@@ -45593,7 +45609,7 @@
       </c>
       <c r="H59" s="7">
         <f>'Estadisticas 1º Vuelta'!G56+'Estadisticas 2º Vuelta'!E59</f>
-        <v>319</v>
+        <v>409</v>
       </c>
       <c r="I59" s="7">
         <f>'Estadisticas 1º Vuelta'!H56+'Estadisticas 2º Vuelta'!F59</f>
@@ -45651,7 +45667,7 @@
       </c>
       <c r="H61" s="7">
         <f>'Estadisticas 1º Vuelta'!G58+'Estadisticas 2º Vuelta'!E61</f>
-        <v>365</v>
+        <v>455</v>
       </c>
       <c r="I61" s="7">
         <f>'Estadisticas 1º Vuelta'!H58+'Estadisticas 2º Vuelta'!F61</f>

</xml_diff>